<commit_message>
Issue with Update-Test-Data noted
The problem files in Update-Test-Data have  aircraft that appear to depart before they have arrived. The file ExampleUpdated10.xlsx has the problem manually fixed, but the others have not been touched.

PlaneModel.py has the following changes:
1.  aircraft.__init__ () now prints an error if an aircraft object is created with departure before arrival.
2. aircraft.over() returns the number of minutes late the aircraft is in departing (0 if it is on time or available earier).
</commit_message>
<xml_diff>
--- a/Update-Test-Data/ExampleUpdated10.xlsx
+++ b/Update-Test-Data/ExampleUpdated10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilu\Navid\EA\EA-Heuristic\Update-Test-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilurquhart/Documents/GitHub/EA-Heuristic/Update-Test-Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124FE098-1A3D-45F8-8EA1-826B2A4F1346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA26501-1D67-1C44-B0A2-F19DB4630593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3010" yWindow="3010" windowWidth="32310" windowHeight="16590" activeTab="2" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
+    <workbookView xWindow="16640" yWindow="3020" windowWidth="22560" windowHeight="14180" xr2:uid="{2111CCAB-A59E-6343-8D75-11A7B1CA366B}"/>
   </bookViews>
   <sheets>
     <sheet name="Aircraft_scheduling" sheetId="1" r:id="rId1"/>
@@ -846,21 +846,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7B622A-250F-6940-8572-A7F426096522}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.08203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.08203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
@@ -883,7 +883,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -894,7 +894,7 @@
         <v>0.2673611111111111</v>
       </c>
       <c r="D2" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E2" s="9">
         <v>0.12736111111111112</v>
@@ -907,7 +907,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>102</v>
@@ -919,7 +919,7 @@
         <v>0.30208333333333331</v>
       </c>
       <c r="D3" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E3" s="9">
         <v>9.2083333333333336E-2</v>
@@ -932,7 +932,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A21" si="1">A3+1</f>
         <v>103</v>
@@ -944,7 +944,7 @@
         <v>0.3576388888888889</v>
       </c>
       <c r="D4" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E4" s="9">
         <v>0.28763888888888889</v>
@@ -957,7 +957,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -969,7 +969,7 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D5" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E5" s="9">
         <v>0.21583333333333332</v>
@@ -982,7 +982,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -994,7 +994,7 @@
         <v>0.46875</v>
       </c>
       <c r="D6" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E6" s="9">
         <v>0.19074074074074074</v>
@@ -1007,7 +1007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1032,7 +1032,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1057,7 +1057,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1069,7 +1069,7 @@
         <v>0.5625</v>
       </c>
       <c r="D9" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E9" s="9">
         <v>0.34049768518518514</v>
@@ -1082,7 +1082,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1094,7 +1094,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D10" s="8">
-        <v>45748</v>
+        <v>45749</v>
       </c>
       <c r="E10" s="9">
         <v>0.36916666666666664</v>
@@ -1107,7 +1107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1132,7 +1132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1157,7 +1157,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1182,7 +1182,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1207,7 +1207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1232,7 +1232,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1257,7 +1257,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1282,7 +1282,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1307,7 +1307,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1332,7 +1332,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1357,7 +1357,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1382,131 +1382,131 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="8"/>
       <c r="D53" s="8"/>
     </row>
@@ -1519,22 +1519,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C9B6E8-A973-BA48-B98B-0A03EAB3C9B6}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="3"/>
     <col min="4" max="4" width="10.83203125" style="4"/>
-    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="94" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -2146,18 +2146,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF47C328-03B3-8E41-ACAA-74BCC13F52C5}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.9140625" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="8"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2539,7 +2539,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>

</xml_diff>